<commit_message>
feat: Update schematics, add mosfet, led ref
</commit_message>
<xml_diff>
--- a/hardware/CompassIO_Project/Project Outputs for CompassIO_Project/BOM/Bill of Materials-CompassIO_Project.xlsx
+++ b/hardware/CompassIO_Project/Project Outputs for CompassIO_Project/BOM/Bill of Materials-CompassIO_Project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="19365"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19980"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-CompassIO_Pro" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="90">
   <si>
     <t>Comment</t>
   </si>
@@ -51,6 +51,24 @@
     <t>RefFournisseur</t>
   </si>
   <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>RAD-0.3</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
     <t>Green LED</t>
   </si>
   <si>
@@ -60,9 +78,6 @@
     <t>D1, D3</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>LED-0</t>
   </si>
   <si>
@@ -78,6 +93,51 @@
     <t>D2</t>
   </si>
   <si>
+    <t>SG90</t>
+  </si>
+  <si>
+    <t>Servo motor</t>
+  </si>
+  <si>
+    <t>MP1</t>
+  </si>
+  <si>
+    <t>MCmall</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>SG90 180 Mini Servo</t>
+  </si>
+  <si>
+    <t>MOSFET-2N7002</t>
+  </si>
+  <si>
+    <t>N-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>ON SEMICONDUCTOR</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>MOSFET-N</t>
+  </si>
+  <si>
+    <t>2N7002</t>
+  </si>
+  <si>
+    <t>2323152</t>
+  </si>
+  <si>
     <t>470</t>
   </si>
   <si>
@@ -96,7 +156,7 @@
     <t>10K</t>
   </si>
   <si>
-    <t>R3</t>
+    <t>R3, R5, R5</t>
   </si>
   <si>
     <t>1K</t>
@@ -105,10 +165,34 @@
     <t>R4</t>
   </si>
   <si>
-    <t>5K</t>
-  </si>
-  <si>
-    <t>R5, R6</t>
+    <t>Resistor 6</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>Resistor 7</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>Resistor 8</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Resistor 9</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>Resistor 11</t>
+  </si>
+  <si>
+    <t>R11</t>
   </si>
   <si>
     <t>Single-Pole, Single-Throw Switch</t>
@@ -129,10 +213,10 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>Factory reset, Reset, Suspend communication</t>
-  </si>
-  <si>
-    <t>S2, S4, S6</t>
+    <t>Factory reset, Reset</t>
+  </si>
+  <si>
+    <t>S2, S4</t>
   </si>
   <si>
     <t>SW-PB</t>
@@ -148,9 +232,6 @@
   </si>
   <si>
     <t>Microchip</t>
-  </si>
-  <si>
-    <t>Farnell</t>
   </si>
   <si>
     <t>RN42-I/RM</t>
@@ -557,7 +638,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -630,7 +711,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
@@ -653,16 +734,16 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>13</v>
@@ -673,28 +754,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="H4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>13</v>
@@ -708,28 +789,28 @@
         <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H5" s="3">
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>13</v>
@@ -737,57 +818,57 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H7" s="3">
         <v>2</v>
@@ -801,25 +882,25 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H8" s="3">
         <v>3</v>
@@ -833,28 +914,28 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H9" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>13</v>
@@ -865,130 +946,354 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="H10" s="3">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="H12" s="3">
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="3">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>62</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Finish schematics bom
</commit_message>
<xml_diff>
--- a/hardware/CompassIO_Project/Project Outputs for CompassIO_Project/BOM/Bill of Materials-CompassIO_Project.xlsx
+++ b/hardware/CompassIO_Project/Project Outputs for CompassIO_Project/BOM/Bill of Materials-CompassIO_Project.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
   <si>
     <t>Comment</t>
   </si>
@@ -78,12 +78,24 @@
     <t>D1, D3</t>
   </si>
   <si>
+    <t>KINGBRIGHT</t>
+  </si>
+  <si>
     <t>LED-0</t>
   </si>
   <si>
+    <t>Farnell</t>
+  </si>
+  <si>
     <t>LED0</t>
   </si>
   <si>
+    <t>KPTD-2012LVZGCK</t>
+  </si>
+  <si>
+    <t>2846598</t>
+  </si>
+  <si>
     <t>Red LED</t>
   </si>
   <si>
@@ -93,6 +105,12 @@
     <t>D2</t>
   </si>
   <si>
+    <t>KPTD-2012LVSURCK</t>
+  </si>
+  <si>
+    <t>2846595</t>
+  </si>
+  <si>
     <t>SG90</t>
   </si>
   <si>
@@ -124,9 +142,6 @@
   </si>
   <si>
     <t>E3</t>
-  </si>
-  <si>
-    <t>Farnell</t>
   </si>
   <si>
     <t>MOSFET-N</t>
@@ -731,86 +746,86 @@
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" s="3">
         <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="H4" s="3">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H5" s="3">
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>13</v>
@@ -818,57 +833,57 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H7" s="3">
         <v>2</v>
@@ -882,25 +897,25 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H8" s="3">
         <v>3</v>
@@ -914,25 +929,25 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -946,25 +961,25 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
@@ -978,25 +993,25 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
@@ -1010,25 +1025,25 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
@@ -1042,25 +1057,25 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
@@ -1074,25 +1089,25 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
@@ -1106,25 +1121,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H15" s="3">
         <v>3</v>
@@ -1138,25 +1153,25 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H16" s="3">
         <v>2</v>
@@ -1170,130 +1185,130 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H19" s="3">
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H20" s="3">
         <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>